<commit_message>
Initial commit, initial files
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1788" uniqueCount="1676">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1793" uniqueCount="1677">
   <si>
     <t>ENGLISH</t>
   </si>
@@ -5054,6 +5054,9 @@
   </si>
   <si>
     <t>Om ni har någonting att invända när det gäller sidans fungering eller tycker ni att det finns några förändringar som kan förenkla att använda sidan, så ska vi gärna höra era anmärkningar och förslag.</t>
+  </si>
+  <si>
+    <t>Browse announcements</t>
   </si>
 </sst>
 </file>
@@ -5351,15 +5354,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E358"/>
+  <dimension ref="A1:E359"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A358" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B359" activeCellId="0" sqref="B359:E359"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.6234817813765"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="110.955465587045"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.8744939271255"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.3724696356275"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="23.6234817813765"/>
@@ -11447,6 +11450,23 @@
       </c>
       <c r="E358" s="10" t="s">
         <v>1675</v>
+      </c>
+    </row>
+    <row r="359" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A359" s="0" t="s">
+        <v>1676</v>
+      </c>
+      <c r="B359" s="7" t="s">
+        <v>1516</v>
+      </c>
+      <c r="C359" s="8" t="s">
+        <v>1517</v>
+      </c>
+      <c r="D359" s="9" t="s">
+        <v>1518</v>
+      </c>
+      <c r="E359" s="10" t="s">
+        <v>1519</v>
       </c>
     </row>
   </sheetData>
@@ -11468,7 +11488,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B359:E359 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -11491,7 +11511,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B359:E359 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>

</xml_diff>